<commit_message>
Finished Setting up EmployeeInfo and Account for entity, repo, service and controller
</commit_message>
<xml_diff>
--- a/documents/1. RD/RD.xlsx
+++ b/documents/1. RD/RD.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherlonetoe/Desktop/hrms/documents/1. RD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christopherlonetoe/Desktop/hrms-v2/documents/1. RD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956D0D1C-18CD-744B-B83D-A2BADF770667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE611E47-2686-5949-9B2D-436698EE93B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" xr2:uid="{625A694E-F168-8945-8042-EFF218857937}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="1" xr2:uid="{625A694E-F168-8945-8042-EFF218857937}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Project Information" sheetId="1" r:id="rId1"/>
+    <sheet name="Authentication" sheetId="2" r:id="rId2"/>
+    <sheet name="Authorization" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Project Name</t>
   </si>
@@ -202,6 +204,33 @@
 - Check-in and Check-out Attendance
 - Submit Overtime Form
 - Can Approve Same Department's Employees' Overtime Form</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>User Registration Form</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>Employee Registration Flow</t>
+  </si>
+  <si>
+    <t>Finished Setting up EmployeeInfo and Account for entity, repo, service and controller</t>
   </si>
 </sst>
 </file>
@@ -305,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -324,16 +353,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -342,14 +371,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -666,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A0CE07-B568-FA48-A759-A0BA176E292E}">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,14 +708,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10">
+      <c r="A1" s="11">
         <v>1</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="17"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="12"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -698,10 +728,10 @@
       <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="17"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="7"/>
@@ -714,10 +744,10 @@
       <c r="N2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="11"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="17"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
@@ -730,14 +760,14 @@
       <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -750,14 +780,14 @@
       <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -770,14 +800,14 @@
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -790,14 +820,14 @@
       <c r="N6" s="7"/>
     </row>
     <row r="7" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="12"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -810,14 +840,14 @@
       <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="11"/>
+      <c r="A8" s="10"/>
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4">
         <v>46038</v>
       </c>
-      <c r="D8" s="17"/>
+      <c r="D8" s="12"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -830,14 +860,14 @@
       <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="17"/>
+      <c r="D9" s="12"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -850,14 +880,14 @@
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="17"/>
+      <c r="D10" s="12"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -870,10 +900,10 @@
       <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
-      <c r="D11" s="17"/>
+      <c r="D11" s="12"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -886,14 +916,14 @@
       <c r="N11" s="7"/>
     </row>
     <row r="12" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10">
+      <c r="A12" s="11">
         <v>2</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="17"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="12"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -906,10 +936,10 @@
       <c r="N12" s="7"/>
     </row>
     <row r="13" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="17"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -922,10 +952,10 @@
       <c r="N13" s="7"/>
     </row>
     <row r="14" spans="1:14" ht="19" x14ac:dyDescent="0.2">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="17"/>
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="12"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -938,12 +968,12 @@
       <c r="N14" s="7"/>
     </row>
     <row r="15" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="11"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -956,10 +986,10 @@
       <c r="N15" s="7"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="12"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
@@ -972,10 +1002,10 @@
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
@@ -988,10 +1018,10 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="12"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
@@ -1004,10 +1034,10 @@
       <c r="N18" s="7"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="11"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="17"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
@@ -1020,14 +1050,14 @@
       <c r="N19" s="7"/>
     </row>
     <row r="20" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10">
+      <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="17"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="12"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
@@ -1040,10 +1070,10 @@
       <c r="N20" s="7"/>
     </row>
     <row r="21" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="17"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
@@ -1056,10 +1086,10 @@
       <c r="N21" s="7"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="17"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="12"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
@@ -1072,12 +1102,12 @@
       <c r="N22" s="7"/>
     </row>
     <row r="23" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="9"/>
+      <c r="B23" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="12"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
@@ -1090,10 +1120,10 @@
       <c r="N23" s="7"/>
     </row>
     <row r="24" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="17"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="12"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
@@ -1106,12 +1136,12 @@
       <c r="N24" s="7"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="9"/>
+      <c r="B25" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="17"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="12"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -1124,12 +1154,12 @@
       <c r="N25" s="7"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="15"/>
-      <c r="B26" s="9" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="17"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
@@ -1142,12 +1172,12 @@
       <c r="N26" s="7"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="15"/>
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="9"/>
+      <c r="B27" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="17"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="12"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
@@ -1160,12 +1190,12 @@
       <c r="N27" s="7"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="9" t="s">
+      <c r="A28" s="9"/>
+      <c r="B28" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="17"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
@@ -1178,12 +1208,12 @@
       <c r="N28" s="7"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="17"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
@@ -1196,12 +1226,12 @@
       <c r="N29" s="7"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="9" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="17"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
@@ -1214,12 +1244,12 @@
       <c r="N30" s="7"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="9" t="s">
+      <c r="A31" s="9"/>
+      <c r="B31" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="17"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="12"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -1232,151 +1262,175 @@
       <c r="N31" s="7"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="15"/>
-      <c r="B32" s="9" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="17"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="12"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="17"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="12"/>
     </row>
     <row r="34" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
-      <c r="B34" s="12" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="12"/>
-      <c r="D34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="12"/>
     </row>
     <row r="35" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="17"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="12"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="9" t="s">
+      <c r="A36" s="9"/>
+      <c r="B36" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="17"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="12"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="9" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="17"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="12"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="9" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="17"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="12"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
-      <c r="B39" s="9" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="17"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="12"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="17"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="12"/>
     </row>
     <row r="41" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10">
+      <c r="A41" s="11">
         <v>4</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C41" s="11"/>
-      <c r="D41" s="15"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="10"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="15"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A43" s="11"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="15"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="11"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="15"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" ht="170" x14ac:dyDescent="0.2">
-      <c r="A45" s="11"/>
+      <c r="A45" s="10"/>
       <c r="B45" t="s">
         <v>14</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D45" s="15"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="289" x14ac:dyDescent="0.2">
-      <c r="A46" s="11"/>
+      <c r="A46" s="10"/>
       <c r="B46" t="s">
         <v>34</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D46" s="15"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" ht="306" x14ac:dyDescent="0.2">
-      <c r="A47" s="11"/>
+      <c r="A47" s="10"/>
       <c r="B47" t="s">
         <v>32</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D47" s="15"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" ht="272" x14ac:dyDescent="0.2">
-      <c r="A48" s="11"/>
+      <c r="A48" s="10"/>
       <c r="B48" t="s">
         <v>37</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="15"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="11"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:C42"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B23:C24"/>
+    <mergeCell ref="B34:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C18"/>
     <mergeCell ref="D41:D49"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="A43:A49"/>
@@ -1393,31 +1447,81 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:C21"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C18"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B23:C24"/>
-    <mergeCell ref="B34:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:C42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8CB2513-33A6-C946-B035-18F65E59003C}">
+  <dimension ref="A2:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="72" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="18">
+        <v>46056</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F8B68A2-F6C3-A441-A454-A63D4D29C56C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>